<commit_message>
Added resting SOC plot
</commit_message>
<xml_diff>
--- a/src/Project Details.xlsx
+++ b/src/Project Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://prevalonenergy-my.sharepoint.com/personal/himanshu_prevalonenergy_com/Documents/I drive/Sizing Tool/System Analytics Tool/deploy_with_render/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="11_F25DC773A252ABDACC1048B2119E5C9C5BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13BAE8F5-4E52-45DD-96B7-95BAC6C76959}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="11_F25DC773A252ABDACC1048B2119E5C9C5BDE58EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03C5EB60-9F58-4EAD-98CA-642CBB3393AA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5650" yWindow="3290" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Project</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>50 MW / 200 MWh</t>
-  </si>
-  <si>
     <t>Application</t>
   </si>
   <si>
@@ -86,9 +80,6 @@
     <t>Nampa, Idaho</t>
   </si>
   <si>
-    <t>82 MW / 328 MWh</t>
-  </si>
-  <si>
     <t>Resource Adequacy</t>
   </si>
   <si>
@@ -102,13 +93,58 @@
   </si>
   <si>
     <t>Happy Valley</t>
+  </si>
+  <si>
+    <t>50 MW</t>
+  </si>
+  <si>
+    <t>82 MW</t>
+  </si>
+  <si>
+    <t>200 MWh</t>
+  </si>
+  <si>
+    <t>328 MWh</t>
+  </si>
+  <si>
+    <t>Rated Power</t>
+  </si>
+  <si>
+    <t>Rated Energy</t>
+  </si>
+  <si>
+    <t>Average Annual Resting SOC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>≤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>50%</t>
+    </r>
+  </si>
+  <si>
+    <t>≤50%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +159,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,10 +187,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,28 +472,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.7265625" customWidth="1"/>
+    <col min="13" max="13" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,102 +503,120 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="F2" s="2">
+        <v>45413</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2">
-        <v>45413</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2">
+      <c r="I2">
         <v>90</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>15</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>380</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="str">
         <f>"-10 deg C to 45 deg C"</f>
         <v>-10 deg C to 45 deg C</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45809</v>
+      </c>
+      <c r="G3" t="str">
+        <f>G2</f>
+        <v>Air Cooled Gen 2 BESS Enclosure</v>
+      </c>
+      <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2">
-        <v>45809</v>
-      </c>
-      <c r="F3" t="str">
-        <f>F2</f>
-        <v>Air Cooled Gen 2 BESS Enclosure</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3">
+      <c r="I3">
         <v>146</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>26</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>365</v>
       </c>
-      <c r="K3" t="str">
+      <c r="L3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="str">
         <f>"-30 deg C to 45 deg C"</f>
         <v>-30 deg C to 45 deg C</v>
       </c>

</xml_diff>